<commit_message>
adding draft overlay and updated spreadsheet.
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-oracle-java-runtime-environment-8-stig-overlay.xlsx
+++ b/cms-ars-3.1-moderate-oracle-java-runtime-environment-8-stig-overlay.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-oracle-java-runtime-environment-8-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C87967BC-AD99-9740-87B8-F2DB7562F632}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0B6F0C1F-48E9-4C47-8A15-E3A0D1D44AEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="67200" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-moderate-oracle-jav" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="119" uniqueCount="98">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="124" uniqueCount="102">
   <si>
     <t>Vuln ID</t>
   </si>
@@ -494,12 +494,24 @@
 NIST SP 800-53 Revision 4 :: SI-2 c
 </t>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Should we make this SC-18 since SC-18(3) isn't in ARS?</t>
+  </si>
+  <si>
+    <t>Should we make this SC-18 since SC-18(4) isn't in ARS?</t>
+  </si>
+  <si>
+    <t>Should we make this SI-2 since SC-2(6) isn't in ARS?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -634,8 +646,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -813,6 +832,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -976,12 +1007,29 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1336,17 +1384,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD18"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="46.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="33.1640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="23.33203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1368,18 +1427,21 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" ht="153" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1392,14 +1454,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" ht="356" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1415,40 +1477,40 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" ht="187" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" ht="221" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1461,17 +1523,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" ht="204" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1484,17 +1546,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1507,14 +1569,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1529,18 +1591,21 @@
       <c r="G8" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="H8" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:8" ht="340" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>48</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -1553,14 +1618,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1575,15 +1640,18 @@
       <c r="G10" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="H10" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:8" ht="356" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1599,14 +1667,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:8" ht="356" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1622,17 +1690,17 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:8" ht="306" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>70</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1645,14 +1713,14 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1668,14 +1736,14 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1690,18 +1758,21 @@
       <c r="G15" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="H15" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>87</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -1713,18 +1784,21 @@
       <c r="G16" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="H16" s="7" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:7" ht="238" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E17" s="1" t="s">

</xml_diff>

<commit_message>
fixed a couple bugs and updated based on EA feedback.
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-oracle-java-runtime-environment-8-stig-overlay.xlsx
+++ b/cms-ars-3.1-moderate-oracle-java-runtime-environment-8-stig-overlay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-oracle-java-runtime-environment-8-unix-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E4D4FCE9-E72A-4A6B-9251-0356E620A6D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C3E27819-861F-204B-BF0F-4765940EBD6E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-moderate-oracle-jav" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="119" uniqueCount="98">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="119" uniqueCount="99">
   <si>
     <t>Vuln ID</t>
   </si>
@@ -494,13 +494,56 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CCI-001162
+The organization establishes implementation guidance for acceptable mobile code and mobile code technologies.
+NIST SP 800-53::SC-18
+NIST SP 800-53A::SC-18
+NIST SP 800-53 Revision 4::SC-18</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">SC-18
+      <t xml:space="preserve">
 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CCI-001695
+The information system prevents the execution of organization-defined unacceptable mobile code.
+NIST SP 800-53 :: SC-18 (3)
+NIST SP 800-53A :: SC-18 (3).1
+NIST SP 800-53 Revision 4 :: SC-18 (3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">
+CCI-001162
+The organization establishes implementation guidance for acceptable mobile code and mobile code technologies.
+NIST SP 800-53::SC-18
+NIST SP 800-53A::SC-18
+NIST SP 800-53 Revision 4::SC-18</t>
     </r>
   </si>
   <si>
@@ -521,13 +564,14 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
       </rPr>
-      <t xml:space="preserve">SC-18
-</t>
+      <t>CCI-001162
+The organization establishes implementation guidance for acceptable mobile code and mobile code technologies.
+NIST SP 800-53::SC-18
+NIST SP 800-53A::SC-18
+NIST SP 800-53 Revision 4::SC-18</t>
     </r>
   </si>
   <si>
@@ -553,7 +597,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">SI-2
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">CCI-001228
+The organization tests software updates related to flaw remediation for effectiveness before installation.
+NIST SP 800-53 Revision 4::SI-2
 </t>
     </r>
   </si>
@@ -562,7 +617,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -704,6 +759,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1088,13 +1148,13 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1454,24 +1514,24 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.34765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.33203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.1484375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.44921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="42.1484375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="46.6484375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="46.1484375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.796875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="23.34765625" style="1"/>
+    <col min="3" max="3" width="36.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="46.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="23.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="34">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1494,7 +1554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="156" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:7" ht="170">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1517,7 +1577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="327.60000000000002" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:7" ht="356">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -1540,7 +1600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="156" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:7" ht="187">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -1563,7 +1623,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="187.2" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:7" ht="221">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -1586,7 +1646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="187.2" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:7" ht="204">
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
@@ -1609,7 +1669,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="280.8" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:7" ht="323">
       <c r="A7" s="4" t="s">
         <v>35</v>
       </c>
@@ -1632,8 +1692,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="280.8" x14ac:dyDescent="0.6">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:7" ht="323">
+      <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1651,11 +1711,11 @@
       <c r="F8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="296.39999999999998" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:7" ht="340">
       <c r="A9" s="6" t="s">
         <v>46</v>
       </c>
@@ -1678,8 +1738,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="296.39999999999998" x14ac:dyDescent="0.6">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:7" ht="323">
+      <c r="A10" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1698,10 +1758,10 @@
         <v>56</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="327.60000000000002" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:7" ht="356">
       <c r="A11" s="4" t="s">
         <v>57</v>
       </c>
@@ -1724,7 +1784,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="327.60000000000002" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:7" ht="356">
       <c r="A12" s="4" t="s">
         <v>63</v>
       </c>
@@ -1747,7 +1807,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="265.2" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:7" ht="306">
       <c r="A13" s="4" t="s">
         <v>67</v>
       </c>
@@ -1770,7 +1830,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="249.6" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:7" ht="289">
       <c r="A14" s="4" t="s">
         <v>73</v>
       </c>
@@ -1793,8 +1853,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="234" x14ac:dyDescent="0.6">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:7" ht="272">
+      <c r="A15" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1813,11 +1873,11 @@
         <v>82</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:7" ht="409.6">
+      <c r="A16" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1835,11 +1895,11 @@
       <c r="F16" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>97</v>
+      <c r="G16" s="8" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="202.8" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:7" ht="238">
       <c r="A17" s="4" t="s">
         <v>88</v>
       </c>

</xml_diff>